<commit_message>
Working forward prop with corner case
Back Prop is started - still needs to be finished and then one
epoch of training will be done.
</commit_message>
<xml_diff>
--- a/NeuralNetwork.xlsx
+++ b/NeuralNetwork.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="180" windowWidth="29600" windowHeight="18200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33440" windowHeight="18180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130404" concurrentCalc="0"/>
+  <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -129,12 +129,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
@@ -233,10 +227,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -568,11 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -619,10 +612,10 @@
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="9"/>
       <c r="C2" s="3">
         <v>0.1</v>
       </c>
@@ -690,10 +683,10 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="5">
         <f>C3+L3</f>
         <v>0.10023886334392688</v>
@@ -764,10 +757,10 @@
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="5">
         <f>C5+L5</f>
         <v>0.10023886334392688</v>
@@ -838,10 +831,10 @@
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="9"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="5">
         <v>0.100238863343927</v>
       </c>
@@ -911,10 +904,10 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="5">
         <v>0.100238863343927</v>
       </c>
@@ -984,10 +977,10 @@
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="5">
         <v>0.100238863343927</v>
       </c>
@@ -1095,10 +1088,10 @@
       </c>
     </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="8"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="3">
         <v>0.1</v>
       </c>
@@ -1166,10 +1159,10 @@
       </c>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="9"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="7">
         <f>C24+L24</f>
         <v>0.10000145560578672</v>
@@ -1240,10 +1233,10 @@
       </c>
     </row>
     <row r="27" spans="1:13">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="9"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="7">
         <f>C26+L26</f>
         <v>0.10000145560578672</v>
@@ -1314,10 +1307,10 @@
       </c>
     </row>
     <row r="29" spans="1:13">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="9"/>
+      <c r="B29" s="8"/>
       <c r="C29" s="7">
         <v>0.100238863343927</v>
       </c>
@@ -1387,10 +1380,10 @@
       </c>
     </row>
     <row r="31" spans="1:13">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="9"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="7">
         <v>0.100238863343927</v>
       </c>
@@ -1460,10 +1453,10 @@
       </c>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="9"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="7">
         <v>0.100238863343927</v>
       </c>
@@ -1531,6 +1524,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A12:B12"/>
@@ -1538,15 +1536,9 @@
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>